<commit_message>
upodate et début compteur
</commit_message>
<xml_diff>
--- a/TNR/TNRSequencer.xlsx
+++ b/TNR/TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -95,7 +95,7 @@
     <t>RO.FOU</t>
   </si>
   <si>
-    <t>RT.ART.001.CRE</t>
+    <t>MP.CPT.001.LEC</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -489,36 +489,20 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>

</xml_diff>